<commit_message>
reformatted some of the sinkholes to be easier for external tools
</commit_message>
<xml_diff>
--- a/Sinkholes_List.xlsx
+++ b/Sinkholes_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="163">
   <si>
     <t>Organization</t>
   </si>
@@ -232,244 +232,277 @@
     <t>Microsoft</t>
   </si>
   <si>
-    <t>131.253.18.11-12</t>
+    <t>199.2.137.0/24</t>
+  </si>
+  <si>
+    <t>https://lists.emergingthreats.net/pipermail/emerging-sigs/2013-June/022148.html</t>
+  </si>
+  <si>
+    <t>204.95.99.59</t>
+  </si>
+  <si>
+    <t>207.46.90.0/24</t>
+  </si>
+  <si>
+    <t>PublicDomainRegistry</t>
+  </si>
+  <si>
+    <t>109.74.196.143</t>
+  </si>
+  <si>
+    <t>Linode</t>
+  </si>
+  <si>
+    <t>50.116.56.144</t>
+  </si>
+  <si>
+    <t>50.116.32.177</t>
+  </si>
+  <si>
+    <t>178.79.190.156</t>
+  </si>
+  <si>
+    <t>Shadowserver</t>
+  </si>
+  <si>
+    <t>87.106.24.200</t>
+  </si>
+  <si>
+    <t>sinkhole-00.shadowserver.org</t>
+  </si>
+  <si>
+    <t>87.106.26.9</t>
+  </si>
+  <si>
+    <t>sinkhole-01.shadowserver.org</t>
+  </si>
+  <si>
+    <t>http://marc.info/?l=emerging-sigs&amp;m=135764068231008&amp;w=2</t>
+  </si>
+  <si>
+    <t>74.208.64.145</t>
+  </si>
+  <si>
+    <t>sinkhole-02.shadowserver.org</t>
+  </si>
+  <si>
+    <t>74.208.64.191</t>
+  </si>
+  <si>
+    <t>sinkhole-03.shadowserver.org</t>
+  </si>
+  <si>
+    <t>74.208.164.166</t>
+  </si>
+  <si>
+    <t>sinkhole-04.shadowserver.org</t>
+  </si>
+  <si>
+    <t>212.227.55.84</t>
+  </si>
+  <si>
+    <t>sinkhole.shadowserver.org</t>
+  </si>
+  <si>
+    <t>74.208.15.160</t>
+  </si>
+  <si>
+    <t>74.208.15.97</t>
+  </si>
+  <si>
+    <t>87.106.250.34</t>
+  </si>
+  <si>
+    <t>87.106.86.28</t>
+  </si>
+  <si>
+    <t>SIDN Labs</t>
+  </si>
+  <si>
+    <t>176.58.104.168</t>
+  </si>
+  <si>
+    <t>sinkhole.sidnlabs.nl</t>
+  </si>
+  <si>
+    <t>sinkhole.DK</t>
+  </si>
+  <si>
+    <t>212.227.20.19</t>
+  </si>
+  <si>
+    <t>sinkhole.dk</t>
+  </si>
+  <si>
+    <t>sinkhole.in</t>
+  </si>
+  <si>
+    <t>86.124.164.25</t>
+  </si>
+  <si>
+    <t>sinkhole.tech</t>
+  </si>
+  <si>
+    <t>79.137.66.14</t>
+  </si>
+  <si>
+    <t>http3.sinkhole.tech</t>
+  </si>
+  <si>
+    <t>95.211.174.92</t>
+  </si>
+  <si>
+    <t>144.217.254.3</t>
+  </si>
+  <si>
+    <t>http4.sinkhole.tech</t>
+  </si>
+  <si>
+    <t>217.182.172.139</t>
+  </si>
+  <si>
+    <t>http1.sinkhole.tech</t>
+  </si>
+  <si>
+    <t>144.217.74.156</t>
+  </si>
+  <si>
+    <t>http2.sinkhole.tech</t>
+  </si>
+  <si>
+    <t>SISRA / Abuse.ch</t>
+  </si>
+  <si>
+    <t>104.155.11.149</t>
+  </si>
+  <si>
+    <t>this-domain-is-sinkholed-by.abuse.ch</t>
+  </si>
+  <si>
+    <t>Spamhaus</t>
+  </si>
+  <si>
+    <t>208.43.245.213</t>
+  </si>
+  <si>
+    <t>sl-reverse.com</t>
+  </si>
+  <si>
+    <t>173.192.192.10</t>
+  </si>
+  <si>
+    <t>199.231.211.108</t>
+  </si>
+  <si>
+    <t>198.98.120.157</t>
+  </si>
+  <si>
+    <t>192.42.116.41</t>
+  </si>
+  <si>
+    <t>87.255.51.229</t>
+  </si>
+  <si>
+    <t>Team Cymru</t>
+  </si>
+  <si>
+    <t>38.102.150.29</t>
+  </si>
+  <si>
+    <t>conficker-sinkhole.net</t>
+  </si>
+  <si>
+    <t>38.229.70.125</t>
+  </si>
+  <si>
+    <t>Torpig-Sinkhole</t>
+  </si>
+  <si>
+    <t>torpig-sinkhole.org</t>
+  </si>
+  <si>
+    <t>87.106.240.162</t>
+  </si>
+  <si>
+    <t>87.106.140.254</t>
+  </si>
+  <si>
+    <t>87.106.141.15</t>
+  </si>
+  <si>
+    <t>Wapack Labs</t>
+  </si>
+  <si>
+    <t>23.253.46.64</t>
+  </si>
+  <si>
+    <t>https://wapacklabs.blogspot.com/2016/07/wapack-labs-sinkhole-results-18.html</t>
+  </si>
+  <si>
+    <t>Zinkhole.org</t>
+  </si>
+  <si>
+    <t>176.31.62.76</t>
+  </si>
+  <si>
+    <t>suspended-domain.org</t>
+  </si>
+  <si>
+    <t>178.32.140.251</t>
+  </si>
+  <si>
+    <t>94.23.175.2</t>
+  </si>
+  <si>
+    <t>OpenDNS</t>
+  </si>
+  <si>
+    <t>146.112.61.104</t>
+  </si>
+  <si>
+    <t>hit-block.opendns.com</t>
+  </si>
+  <si>
+    <t>https://support.opendns.com/hc/en-us/articles/227986927-What-are-the-Cisco-Umbrella-Block-Page-IP-Addresses-</t>
+  </si>
+  <si>
+    <t>146.112.61.105</t>
+  </si>
+  <si>
+    <t>hit-botnet.opendns.com</t>
+  </si>
+  <si>
+    <t>146.112.61.106</t>
+  </si>
+  <si>
+    <t>hit-adult.opendns.com</t>
+  </si>
+  <si>
+    <t>146.112.61.107</t>
+  </si>
+  <si>
+    <t>hit-malware.opendns.com</t>
+  </si>
+  <si>
+    <t>146.112.61.108</t>
+  </si>
+  <si>
+    <t>hit-phish.opendns.com</t>
+  </si>
+  <si>
+    <t>146.112.61.109</t>
+  </si>
+  <si>
+    <t>146.112.61.110</t>
+  </si>
+  <si>
+    <t>131.253.18.11</t>
   </si>
   <si>
     <t>http://doc.emergingthreats.net/bin/view/Main/2016101</t>
   </si>
   <si>
-    <t>199.2.137.0/24</t>
-  </si>
-  <si>
-    <t>https://lists.emergingthreats.net/pipermail/emerging-sigs/2013-June/022148.html</t>
-  </si>
-  <si>
-    <t>204.95.99.59</t>
-  </si>
-  <si>
-    <t>207.46.90.0/24</t>
-  </si>
-  <si>
-    <t>PublicDomainRegistry</t>
-  </si>
-  <si>
-    <t>109.74.196.143</t>
-  </si>
-  <si>
-    <t>Linode</t>
-  </si>
-  <si>
-    <t>50.116.56.144</t>
-  </si>
-  <si>
-    <t>50.116.32.177</t>
-  </si>
-  <si>
-    <t>178.79.190.156</t>
-  </si>
-  <si>
-    <t>Shadowserver</t>
-  </si>
-  <si>
-    <t>87.106.24.200</t>
-  </si>
-  <si>
-    <t>sinkhole-00.shadowserver.org</t>
-  </si>
-  <si>
-    <t>87.106.26.9</t>
-  </si>
-  <si>
-    <t>sinkhole-01.shadowserver.org</t>
-  </si>
-  <si>
-    <t>http://marc.info/?l=emerging-sigs&amp;m=135764068231008&amp;w=2</t>
-  </si>
-  <si>
-    <t>74.208.64.145</t>
-  </si>
-  <si>
-    <t>sinkhole-02.shadowserver.org</t>
-  </si>
-  <si>
-    <t>74.208.64.191</t>
-  </si>
-  <si>
-    <t>sinkhole-03.shadowserver.org</t>
-  </si>
-  <si>
-    <t>74.208.164.166</t>
-  </si>
-  <si>
-    <t>sinkhole-04.shadowserver.org</t>
-  </si>
-  <si>
-    <t>212.227.55.84</t>
-  </si>
-  <si>
-    <t>sinkhole.shadowserver.org</t>
-  </si>
-  <si>
-    <t>74.208.15.160</t>
-  </si>
-  <si>
-    <t>74.208.15.97</t>
-  </si>
-  <si>
-    <t>87.106.250.34</t>
-  </si>
-  <si>
-    <t>87.106.86.28</t>
-  </si>
-  <si>
-    <t>SIDN Labs</t>
-  </si>
-  <si>
-    <t>176.58.104.168</t>
-  </si>
-  <si>
-    <t>sinkhole.sidnlabs.nl</t>
-  </si>
-  <si>
-    <t>sinkhole.DK</t>
-  </si>
-  <si>
-    <t>212.227.20.19</t>
-  </si>
-  <si>
-    <t>sinkhole.dk</t>
-  </si>
-  <si>
-    <t>sinkhole.in</t>
-  </si>
-  <si>
-    <t>86.124.164.25</t>
-  </si>
-  <si>
-    <t>sinkhole.tech</t>
-  </si>
-  <si>
-    <t>79.137.66.14</t>
-  </si>
-  <si>
-    <t>http3.sinkhole.tech</t>
-  </si>
-  <si>
-    <t>95.211.174.92</t>
-  </si>
-  <si>
-    <t>144.217.254.3</t>
-  </si>
-  <si>
-    <t>http4.sinkhole.tech</t>
-  </si>
-  <si>
-    <t>217.182.172.139</t>
-  </si>
-  <si>
-    <t>http1.sinkhole.tech</t>
-  </si>
-  <si>
-    <t>144.217.74.156</t>
-  </si>
-  <si>
-    <t>http2.sinkhole.tech</t>
-  </si>
-  <si>
-    <t>SISRA / Abuse.ch</t>
-  </si>
-  <si>
-    <t>104.155.11.149</t>
-  </si>
-  <si>
-    <t>this-domain-is-sinkholed-by.abuse.ch</t>
-  </si>
-  <si>
-    <t>Spamhaus</t>
-  </si>
-  <si>
-    <t>208.43.245.213</t>
-  </si>
-  <si>
-    <t>sl-reverse.com</t>
-  </si>
-  <si>
-    <t>173.192.192.10</t>
-  </si>
-  <si>
-    <t>199.231.211.108</t>
-  </si>
-  <si>
-    <t>198.98.120.157</t>
-  </si>
-  <si>
-    <t>192.42.116.41</t>
-  </si>
-  <si>
-    <t>87.255.51.229</t>
-  </si>
-  <si>
-    <t>Team Cymru</t>
-  </si>
-  <si>
-    <t>38.102.150.29</t>
-  </si>
-  <si>
-    <t>conficker-sinkhole.net</t>
-  </si>
-  <si>
-    <t>38.229.70.125</t>
-  </si>
-  <si>
-    <t>Torpig-Sinkhole</t>
-  </si>
-  <si>
-    <t>torpig-sinkhole.org</t>
-  </si>
-  <si>
-    <t>87.106.240.162</t>
-  </si>
-  <si>
-    <t>87.106.140.254</t>
-  </si>
-  <si>
-    <t>87.106.141.15</t>
-  </si>
-  <si>
-    <t>Wapack Labs</t>
-  </si>
-  <si>
-    <t>23.253.46.64</t>
-  </si>
-  <si>
-    <t>https://wapacklabs.blogspot.com/2016/07/wapack-labs-sinkhole-results-18.html</t>
-  </si>
-  <si>
-    <t>Zinkhole.org</t>
-  </si>
-  <si>
-    <t>176.31.62.76</t>
-  </si>
-  <si>
-    <t>suspended-domain.org</t>
-  </si>
-  <si>
-    <t>178.32.140.251</t>
-  </si>
-  <si>
-    <t>94.23.175.2</t>
-  </si>
-  <si>
-    <t>OpenDNS</t>
-  </si>
-  <si>
-    <t>146.112.61.104-110</t>
-  </si>
-  <si>
-    <t>hit-{block,botnet,adult,malware,phish,block,malware}.opendns.com</t>
-  </si>
-  <si>
-    <t>https://support.opendns.com/hc/en-us/articles/227986927-What-are-the-Cisco-Umbrella-Block-Page-IP-Addresses-</t>
+    <t>131.253.18.12</t>
   </si>
 </sst>
 </file>
@@ -814,7 +847,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1152,7 +1185,7 @@
         <v>71</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1160,38 +1193,38 @@
         <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29" t="s">
         <v>71</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
         <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
+      </c>
+      <c r="D30" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D31" t="s">
         <v>52</v>
@@ -1199,13 +1232,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" t="s">
         <v>78</v>
-      </c>
-      <c r="B32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C32" t="s">
-        <v>80</v>
       </c>
       <c r="D32" t="s">
         <v>52</v>
@@ -1213,13 +1246,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
         <v>78</v>
-      </c>
-      <c r="B33" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" t="s">
-        <v>80</v>
       </c>
       <c r="D33" t="s">
         <v>52</v>
@@ -1227,21 +1260,18 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
         <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s">
         <v>85</v>
@@ -1249,24 +1279,24 @@
       <c r="C35" t="s">
         <v>86</v>
       </c>
+      <c r="D35" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
         <v>90</v>
@@ -1277,7 +1307,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B38" t="s">
         <v>92</v>
@@ -1288,7 +1318,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
         <v>94</v>
@@ -1299,85 +1329,85 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
         <v>96</v>
       </c>
       <c r="C40" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C42" t="s">
-        <v>97</v>
+        <v>95</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C43" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="B44" t="s">
         <v>101</v>
       </c>
       <c r="C44" t="s">
-        <v>97</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B45" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C45" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B46" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" t="s">
         <v>106</v>
-      </c>
-      <c r="C46" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1388,34 +1418,34 @@
         <v>109</v>
       </c>
       <c r="C47" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B48" t="s">
         <v>111</v>
       </c>
       <c r="C48" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B49" t="s">
+        <v>112</v>
+      </c>
+      <c r="C49" t="s">
         <v>113</v>
-      </c>
-      <c r="C49" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B50" t="s">
         <v>114</v>
@@ -1426,7 +1456,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B51" t="s">
         <v>116</v>
@@ -1437,214 +1467,315 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B52" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C52" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B53" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C53" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B54" t="s">
         <v>124</v>
       </c>
       <c r="C54" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
+        <v>121</v>
+      </c>
+      <c r="B55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C55" t="s">
         <v>123</v>
-      </c>
-      <c r="B55" t="s">
-        <v>126</v>
-      </c>
-      <c r="C55" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
+        <v>121</v>
+      </c>
+      <c r="B56" t="s">
+        <v>126</v>
+      </c>
+      <c r="C56" t="s">
         <v>123</v>
-      </c>
-      <c r="B56" t="s">
-        <v>127</v>
-      </c>
-      <c r="C56" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" t="s">
+        <v>127</v>
+      </c>
+      <c r="C57" t="s">
         <v>123</v>
-      </c>
-      <c r="B57" t="s">
-        <v>128</v>
-      </c>
-      <c r="C57" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" t="s">
+        <v>128</v>
+      </c>
+      <c r="C58" t="s">
         <v>123</v>
-      </c>
-      <c r="B58" t="s">
-        <v>129</v>
-      </c>
-      <c r="C58" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B59" t="s">
         <v>130</v>
       </c>
       <c r="C59" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B60" t="s">
         <v>132</v>
       </c>
       <c r="C60" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B61" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" t="s">
         <v>134</v>
-      </c>
-      <c r="C61" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" t="s">
         <v>135</v>
       </c>
-      <c r="B62" t="s">
-        <v>96</v>
-      </c>
       <c r="C62" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B63" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C63" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B64" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C64" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B65" t="s">
         <v>139</v>
       </c>
-      <c r="C65" t="s">
-        <v>136</v>
+      <c r="D65" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B66" t="s">
-        <v>141</v>
-      </c>
-      <c r="D66" s="1" t="s">
         <v>142</v>
+      </c>
+      <c r="C66" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B67" t="s">
         <v>144</v>
       </c>
       <c r="C67" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68" t="s">
         <v>143</v>
-      </c>
-      <c r="B68" t="s">
-        <v>146</v>
-      </c>
-      <c r="C68" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B69" t="s">
         <v>147</v>
       </c>
       <c r="C69" t="s">
-        <v>145</v>
+        <v>148</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
+        <v>146</v>
+      </c>
+      <c r="B70" t="s">
+        <v>150</v>
+      </c>
+      <c r="C70" t="s">
+        <v>151</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>146</v>
+      </c>
+      <c r="B71" t="s">
+        <v>152</v>
+      </c>
+      <c r="C71" t="s">
+        <v>153</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>146</v>
+      </c>
+      <c r="B72" t="s">
+        <v>154</v>
+      </c>
+      <c r="C72" t="s">
+        <v>155</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>146</v>
+      </c>
+      <c r="B73" t="s">
+        <v>156</v>
+      </c>
+      <c r="C73" t="s">
+        <v>157</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" t="s">
+        <v>158</v>
+      </c>
+      <c r="C74" t="s">
         <v>148</v>
       </c>
-      <c r="B70" t="s">
+      <c r="D74" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C70" t="s">
-        <v>150</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>151</v>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>146</v>
+      </c>
+      <c r="B75" t="s">
+        <v>159</v>
+      </c>
+      <c r="C75" t="s">
+        <v>155</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>71</v>
+      </c>
+      <c r="B76" t="s">
+        <v>160</v>
+      </c>
+      <c r="C76" t="s">
+        <v>71</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>71</v>
+      </c>
+      <c r="B77" t="s">
+        <v>162</v>
+      </c>
+      <c r="C77" t="s">
+        <v>71</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1657,12 +1788,19 @@
     <hyperlink ref="D27" r:id="rId6"/>
     <hyperlink ref="D28" r:id="rId7"/>
     <hyperlink ref="D29" r:id="rId8"/>
-    <hyperlink ref="D30" r:id="rId9"/>
-    <hyperlink ref="D36" r:id="rId10"/>
+    <hyperlink ref="D35" r:id="rId9"/>
+    <hyperlink ref="D42" r:id="rId10"/>
     <hyperlink ref="D43" r:id="rId11"/>
-    <hyperlink ref="D44" r:id="rId12"/>
-    <hyperlink ref="D66" r:id="rId13"/>
+    <hyperlink ref="D65" r:id="rId12"/>
+    <hyperlink ref="D69" r:id="rId13"/>
     <hyperlink ref="D70" r:id="rId14"/>
+    <hyperlink ref="D71" r:id="rId15"/>
+    <hyperlink ref="D72" r:id="rId16"/>
+    <hyperlink ref="D73" r:id="rId17"/>
+    <hyperlink ref="D74" r:id="rId18"/>
+    <hyperlink ref="D75" r:id="rId19"/>
+    <hyperlink ref="D76" r:id="rId20"/>
+    <hyperlink ref="D77" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added in IANA blackhole servers
</commit_message>
<xml_diff>
--- a/Sinkholes_List.xlsx
+++ b/Sinkholes_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="171">
   <si>
     <t>Organization</t>
   </si>
@@ -503,6 +503,30 @@
   </si>
   <si>
     <t>131.253.18.12</t>
+  </si>
+  <si>
+    <t>IANA</t>
+  </si>
+  <si>
+    <t>192.175.48.6</t>
+  </si>
+  <si>
+    <t>blackhole-1.iana.org</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Blackhole_server</t>
+  </si>
+  <si>
+    <t>192.175.48.42</t>
+  </si>
+  <si>
+    <t>blackhole-2.iana.org</t>
+  </si>
+  <si>
+    <t>192.175.48.1</t>
+  </si>
+  <si>
+    <t>prisoner.iana.org</t>
   </si>
 </sst>
 </file>
@@ -847,7 +871,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1776,6 +1800,48 @@
       </c>
       <c r="D77" s="1" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>163</v>
+      </c>
+      <c r="B78" t="s">
+        <v>164</v>
+      </c>
+      <c r="C78" t="s">
+        <v>165</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>163</v>
+      </c>
+      <c r="B79" t="s">
+        <v>167</v>
+      </c>
+      <c r="C79" t="s">
+        <v>168</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>163</v>
+      </c>
+      <c r="B80" t="s">
+        <v>169</v>
+      </c>
+      <c r="C80" t="s">
+        <v>170</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1801,6 +1867,9 @@
     <hyperlink ref="D75" r:id="rId19"/>
     <hyperlink ref="D76" r:id="rId20"/>
     <hyperlink ref="D77" r:id="rId21"/>
+    <hyperlink ref="D78" r:id="rId22"/>
+    <hyperlink ref="D79" r:id="rId23"/>
+    <hyperlink ref="D80" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add CNCERT/CC sinkhole IP
</commit_message>
<xml_diff>
--- a/Sinkholes_List.xlsx
+++ b/Sinkholes_List.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="159">
   <si>
     <t>Organization</t>
   </si>
@@ -483,6 +483,15 @@
   </si>
   <si>
     <t>https://github.com/grettir/malware-sinkholes/blob/905841db3b3cd86052d577c137ac9868c92dcb3b/malware_sinkholes.txt#L256</t>
+  </si>
+  <si>
+    <t>CNCERT/CC</t>
+  </si>
+  <si>
+    <t>183.236.2.18</t>
+  </si>
+  <si>
+    <t>China Mobile communications corporation</t>
   </si>
 </sst>
 </file>
@@ -1717,6 +1726,18 @@
         <v>155</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>156</v>
+      </c>
+      <c r="B72" t="s">
+        <v>157</v>
+      </c>
+      <c r="C72" t="s">
+        <v>158</v>
+      </c>
+      <c r="D72" t="s"/>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Add CNCERT/CC sinkhole IP"
This reverts commit c87970b2a11a28e77c14fbdd4ad7c3927531f7f2.
</commit_message>
<xml_diff>
--- a/Sinkholes_List.xlsx
+++ b/Sinkholes_List.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="156">
   <si>
     <t>Organization</t>
   </si>
@@ -483,15 +483,6 @@
   </si>
   <si>
     <t>https://github.com/grettir/malware-sinkholes/blob/905841db3b3cd86052d577c137ac9868c92dcb3b/malware_sinkholes.txt#L256</t>
-  </si>
-  <si>
-    <t>CNCERT/CC</t>
-  </si>
-  <si>
-    <t>183.236.2.18</t>
-  </si>
-  <si>
-    <t>China Mobile communications corporation</t>
   </si>
 </sst>
 </file>
@@ -1726,18 +1717,6 @@
         <v>155</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" t="s">
-        <v>156</v>
-      </c>
-      <c r="B72" t="s">
-        <v>157</v>
-      </c>
-      <c r="C72" t="s">
-        <v>158</v>
-      </c>
-      <c r="D72" t="s"/>
-    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add CNCERT/CC sinkhole IP (#12)
* Add CNCERT/CC sinkhole IP

* Revert "Add CNCERT/CC sinkhole IP"

This reverts commit c87970b2a11a28e77c14fbdd4ad7c3927531f7f2.

* Add CNCERT/CC sinkhole IP
</commit_message>
<xml_diff>
--- a/Sinkholes_List.xlsx
+++ b/Sinkholes_List.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="159">
   <si>
     <t>Organization</t>
   </si>
@@ -483,6 +483,15 @@
   </si>
   <si>
     <t>https://github.com/grettir/malware-sinkholes/blob/905841db3b3cd86052d577c137ac9868c92dcb3b/malware_sinkholes.txt#L256</t>
+  </si>
+  <si>
+    <t>CNCERT/CC</t>
+  </si>
+  <si>
+    <t>183.236.2.18</t>
+  </si>
+  <si>
+    <t>China Mobile communications corporation</t>
   </si>
 </sst>
 </file>
@@ -1717,6 +1726,18 @@
         <v>155</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>156</v>
+      </c>
+      <c r="B72" t="s">
+        <v>157</v>
+      </c>
+      <c r="C72" t="s">
+        <v>158</v>
+      </c>
+      <c r="D72" t="s"/>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>